<commit_message>
Updated tutorial voor evaluation additional rules
1 tutorial for ARS and QRS
</commit_message>
<xml_diff>
--- a/solvency2-rules/ars_patterns_additional_rules.xlsx
+++ b/solvency2-rules/ars_patterns_additional_rules.xlsx
@@ -1369,10 +1369,10 @@
     <t>IF {"S.15.01.01.01,C0040"}!=None THEN {"S.15.01.01.01,C0050"} != None</t>
   </si>
   <si>
-    <t>IF {"S.15.01.01.01,C0040"}!=None THEN {"S.15.01.01.01,C0070"} &gt;0</t>
-  </si>
-  <si>
-    <t>IF {"S.15.01.01.01,C0040"}!=None THEN {"S.15.01.01.01,C0080"} &gt;0</t>
+    <t>IF {"S.15.01.01.01,C0040"}!=None THEN {"S.15.01.01.01,C0070"} != None</t>
+  </si>
+  <si>
+    <t>IF {"S.15.01.01.01,C0040"}!=None THEN {"S.15.01.01.01,C0080"} != None</t>
   </si>
   <si>
     <t>IF {"S.15.01.01.01,C0040"}!=None THEN {"S.15.01.01.01,C0090"} != 0</t>
@@ -1474,10 +1474,10 @@
     <t>IF {"S.23.04.01.02,C0185"} != None THEN {"S.23.04.01.02,C0200"} &gt; 0</t>
   </si>
   <si>
-    <t>IF {"S.23.04.01.02,C0185"} != None THEN {"S.23.04.01.02,C0210"} &gt; 0</t>
-  </si>
-  <si>
-    <t>IF {"S.23.04.01.02,C0185"} != None THEN {"S.23.04.01.02,C0230"} &gt;0</t>
+    <t>IF {"S.23.04.01.02,C0185"} != None THEN {"S.23.04.01.02,C0210"} != None</t>
+  </si>
+  <si>
+    <t>IF {"S.23.04.01.02,C0185"} != None THEN {"S.23.04.01.02,C0230"} != None</t>
   </si>
   <si>
     <t>IF {"S.23.04.01.03,C0265"} != None THEN {"S.23.04.01.03,C0270"} != None</t>
@@ -1513,7 +1513,7 @@
     <t>IF {"S.23.04.01.04,C0445"} != None THEN {"S.23.04.01.04,C0480"} &gt; 0 | {"S.23.04.01.04,C0490"} &gt; 0 | {"S.23.04.01.04,C0500"} &gt; 0</t>
   </si>
   <si>
-    <t>IF {"S.23.04.01.04,C0445"} != None THEN {"S.23.04.01.04,C0510"} &gt; 0</t>
+    <t>IF {"S.23.04.01.04,C0445"} != None THEN {"S.23.04.01.04,C0510"} != None</t>
   </si>
   <si>
     <t>IF {"S.23.04.01.05,C0565"} != None THEN {"S.23.04.01.05,C0570"} != None</t>
@@ -2611,10 +2611,10 @@
     <t>df[(df['S.15.01.01.01,C0040']!=None) &amp; (df['S.15.01.01.01,C0050']!=None)]</t>
   </si>
   <si>
-    <t>df[(df['S.15.01.01.01,C0040']!=None) &amp; (df['S.15.01.01.01,C0070']&gt;0)]</t>
-  </si>
-  <si>
-    <t>df[(df['S.15.01.01.01,C0040']!=None) &amp; (df['S.15.01.01.01,C0080']&gt;0)]</t>
+    <t>df[(df['S.15.01.01.01,C0040']!=None) &amp; (df['S.15.01.01.01,C0070']!=None)]</t>
+  </si>
+  <si>
+    <t>df[(df['S.15.01.01.01,C0040']!=None) &amp; (df['S.15.01.01.01,C0080']!=None)]</t>
   </si>
   <si>
     <t>df[(df['S.15.01.01.01,C0040']!=None) &amp; (df['S.15.01.01.01,C0090']!=0)]</t>
@@ -2716,10 +2716,10 @@
     <t>df[(df['S.23.04.01.02,C0185']!=None) &amp; (df['S.23.04.01.02,C0200']&gt;0)]</t>
   </si>
   <si>
-    <t>df[(df['S.23.04.01.02,C0185']!=None) &amp; (df['S.23.04.01.02,C0210']&gt;0)]</t>
-  </si>
-  <si>
-    <t>df[(df['S.23.04.01.02,C0185']!=None) &amp; (df['S.23.04.01.02,C0230']&gt;0)]</t>
+    <t>df[(df['S.23.04.01.02,C0185']!=None) &amp; (df['S.23.04.01.02,C0210']!=None)]</t>
+  </si>
+  <si>
+    <t>df[(df['S.23.04.01.02,C0185']!=None) &amp; (df['S.23.04.01.02,C0230']!=None)]</t>
   </si>
   <si>
     <t>df[(df['S.23.04.01.03,C0265']!=None) &amp; (df['S.23.04.01.03,C0270']!=None)]</t>
@@ -2755,7 +2755,7 @@
     <t>df[(df['S.23.04.01.04,C0445']!=None) &amp; (((df['S.23.04.01.04,C0480']&gt;0) | (df['S.23.04.01.04,C0490']&gt;0)) | (df['S.23.04.01.04,C0500']&gt;0))]</t>
   </si>
   <si>
-    <t>df[(df['S.23.04.01.04,C0445']!=None) &amp; (df['S.23.04.01.04,C0510']&gt;0)]</t>
+    <t>df[(df['S.23.04.01.04,C0445']!=None) &amp; (df['S.23.04.01.04,C0510']!=None)]</t>
   </si>
   <si>
     <t>df[(df['S.23.04.01.05,C0565']!=None) &amp; (df['S.23.04.01.05,C0570']!=None)]</t>
@@ -3841,10 +3841,10 @@
     <t>df[(df['S.15.01.01.01,C0040']!=None) &amp; ~(df['S.15.01.01.01,C0050']!=None)]</t>
   </si>
   <si>
-    <t>df[(df['S.15.01.01.01,C0040']!=None) &amp; ~(df['S.15.01.01.01,C0070']&gt;0)]</t>
-  </si>
-  <si>
-    <t>df[(df['S.15.01.01.01,C0040']!=None) &amp; ~(df['S.15.01.01.01,C0080']&gt;0)]</t>
+    <t>df[(df['S.15.01.01.01,C0040']!=None) &amp; ~(df['S.15.01.01.01,C0070']!=None)]</t>
+  </si>
+  <si>
+    <t>df[(df['S.15.01.01.01,C0040']!=None) &amp; ~(df['S.15.01.01.01,C0080']!=None)]</t>
   </si>
   <si>
     <t>df[(df['S.15.01.01.01,C0040']!=None) &amp; ~(df['S.15.01.01.01,C0090']!=0)]</t>
@@ -3946,10 +3946,10 @@
     <t>df[(df['S.23.04.01.02,C0185']!=None) &amp; ~(df['S.23.04.01.02,C0200']&gt;0)]</t>
   </si>
   <si>
-    <t>df[(df['S.23.04.01.02,C0185']!=None) &amp; ~(df['S.23.04.01.02,C0210']&gt;0)]</t>
-  </si>
-  <si>
-    <t>df[(df['S.23.04.01.02,C0185']!=None) &amp; ~(df['S.23.04.01.02,C0230']&gt;0)]</t>
+    <t>df[(df['S.23.04.01.02,C0185']!=None) &amp; ~(df['S.23.04.01.02,C0210']!=None)]</t>
+  </si>
+  <si>
+    <t>df[(df['S.23.04.01.02,C0185']!=None) &amp; ~(df['S.23.04.01.02,C0230']!=None)]</t>
   </si>
   <si>
     <t>df[(df['S.23.04.01.03,C0265']!=None) &amp; ~(df['S.23.04.01.03,C0270']!=None)]</t>
@@ -3985,7 +3985,7 @@
     <t>df[(df['S.23.04.01.04,C0445']!=None) &amp; ~(((df['S.23.04.01.04,C0480']&gt;0) | (df['S.23.04.01.04,C0490']&gt;0)) | (df['S.23.04.01.04,C0500']&gt;0))]</t>
   </si>
   <si>
-    <t>df[(df['S.23.04.01.04,C0445']!=None) &amp; ~(df['S.23.04.01.04,C0510']&gt;0)]</t>
+    <t>df[(df['S.23.04.01.04,C0445']!=None) &amp; ~(df['S.23.04.01.04,C0510']!=None)]</t>
   </si>
   <si>
     <t>df[(df['S.23.04.01.05,C0565']!=None) &amp; ~(df['S.23.04.01.05,C0570']!=None)]</t>

</xml_diff>